<commit_message>
Updated Risk Managment Log
Updated Risk Log per Michelles reiview
</commit_message>
<xml_diff>
--- a/Risk mangaement Log.xlsx
+++ b/Risk mangaement Log.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PeacheyMacbook/Google Drive/Uni/ITC303 - Dev 1/Asses2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PeacheyMacbook/Google Drive/Uni/Development-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="32900" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="460" windowWidth="32900" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -730,6 +730,24 @@
   </si>
   <si>
     <t xml:space="preserve">*note: Any additional risks that come up in iteration plan meetings must be reported to this document. Conversly, any risks that are added to this plan must be brought up in iteration plan meetings. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project scope has not been clearly identified. Group members are currently completing tasks without a succient project vision. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wuthout a common vision all team members are currently developing based on their own understanding of the project. This could lead to inconsistant work being completed among members, affecting the outcome of the project. </t>
+  </si>
+  <si>
+    <t>Project Planning, Project Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parts of assignments are being completed without the vision document being completed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As part of Assignment 1. A project vision will be submitted and distributed to team members throughout its development. This will give all group members the same goal when writing their documentation. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly meetings are being held to keep eveyrone accoutable for their work. Minimising any long term effects with not having this document. </t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1077,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1084,9 +1102,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1681,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1698,23 +1713,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="27" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1771,125 +1786,146 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="55" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="33" t="s">
+      <c r="I8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="13"/>
+      <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:13" ht="55" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="22" t="s">
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="32" t="s">
+      <c r="J9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="M9" s="33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+    <row r="10" spans="1:13" ht="55" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8" t="str">
-        <f t="shared" ref="E10:E12" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
-        <v/>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="35"/>
+      <c r="B10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="34" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E10:E12" si="0">IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
         <v/>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="6"/>
@@ -1899,22 +1935,22 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="20"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1935,7 +1971,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L10:L12">
+  <conditionalFormatting sqref="L11:L12">
     <cfRule type="cellIs" dxfId="13" priority="10" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -1988,7 +2024,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L10:L12 C8:D12 E9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9 C8:D12 L11:L12">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K12">

</xml_diff>

<commit_message>
with comments from col
</commit_message>
<xml_diff>
--- a/Risk mangaement Log.xlsx
+++ b/Risk mangaement Log.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PeacheyMacbook/Google Drive/Uni/Development-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="32900" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="705" yWindow="465" windowWidth="32895" windowHeight="16875" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="Risk_Area">[1]DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,11 +32,60 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>McKeahnie, Collin</author>
     <author>eze3</author>
     <author>e</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This needs to be finished</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+There are quite a lot of spelling mistakes through out the document. Spell check should pick them up</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +171,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Here would it be better to have a title or name for the risk. 
+At a glance it is hard to tell what the risks are.
+For example risk 1 could be called 'server unavalible' or something</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1">
+    <comment ref="F7" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -371,7 +446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0">
+    <comment ref="G7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -394,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="1">
+    <comment ref="H7" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0">
+    <comment ref="I7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -440,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J7" authorId="1">
+    <comment ref="J7" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -463,7 +538,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K7" authorId="1">
+    <comment ref="K7" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -486,7 +561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L7" authorId="1">
+    <comment ref="L7" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M7" authorId="0">
+    <comment ref="M7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -532,7 +607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N7" authorId="1">
+    <comment ref="N7" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -552,6 +627,225 @@
             <family val="2"/>
           </rPr>
           <t>This column should be populated with a description of the risk contingency plan.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is not a description of the risk. The risk, if I understand correctly, is the server is unavalible and the description should be something about the user trying to start a game but has no questions or finish a game but cannot upload gamedata
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The impact of this risk on the project is the game will not run in multiplayer mode. If at start up the server is down the user will be presented with a pop up notification if at the end of a game the gamedata will be stored locally and uploaded at a later date (I just made that up change it as you want, but the impact has to be a clear thing that will happen if this risk occours)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Is this risk not in 'game play' or 'functionallity' or something? The actual architecture of the game wiill not be affected by the server being unreachable for a period of time</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">McKeahnie, Collin:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hostinger will inform the development team if the server is down as a result of an error at their end or if we need to adjust or servie plan to keep up with traffic demands</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A trigger is something that may cause this risk to occure. In this case the trigger would be, the user has no internet access, our hosting company goes down or exessive traffic causes server errors</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+"….If the current service plan proves to…."
+also we are renting this space, its cheap but I do pay them
+This is really the contingency plan. Realistically our respons to a server crash is do nothing and wait it out.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+We now have a vision doc so is this closed?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bold?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>McKeahnie, Collin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Delete this and comments from the document</t>
         </r>
       </text>
     </comment>
@@ -756,11 +1050,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -841,6 +1135,32 @@
       <sz val="8"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1317,6 +1637,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1325,110 +1648,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="Risk_Tracking_Log"/>
       <sheetName val="DropDown_Elements"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Schedule</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Initial Costs</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Life-cycle Costs</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Technical Obsolescence</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Feasibility</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Reliability of Systems</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Dependencies/Interoperability</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Surety Considerations</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Future Procurements</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Project Management</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Overall Project Failure</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>Organizational/Change Management</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Business</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Data/Information</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Technology</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>Strategic</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>Security</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Privacy</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>Project Resources</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1699,23 +1922,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
-    <col min="2" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="3" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="5" width="13.875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.33203125" customWidth="1"/>
-    <col min="10" max="14" width="30.33203125" customWidth="1"/>
+    <col min="7" max="8" width="30.375" customWidth="1"/>
+    <col min="9" max="9" width="23.375" customWidth="1"/>
+    <col min="10" max="14" width="30.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>25</v>
       </c>
@@ -1737,18 +1960,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" ht="23" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:14" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +2015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="55" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>20</v>
       </c>
@@ -1832,7 +2055,7 @@
       </c>
       <c r="N8" s="12"/>
     </row>
-    <row r="9" spans="1:14" ht="55" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>21</v>
       </c>
@@ -1874,7 +2097,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="55" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>22</v>
       </c>
@@ -1914,7 +2137,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>23</v>
       </c>
@@ -1935,7 +2158,7 @@
       <c r="M11" s="16"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>24</v>
       </c>
@@ -1956,17 +2179,17 @@
       <c r="M12" s="13"/>
       <c r="N12" s="19"/>
     </row>
-    <row r="15" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2050,6 +2273,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>